<commit_message>
feat:done laporan data online indera dan bug fix laporan
</commit_message>
<xml_diff>
--- a/public/assets/report/report-afp.xlsx
+++ b/public/assets/report/report-afp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\sistem-pelaporan-terpadu-puskesmas\public\assets\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588BFDDB-A657-446B-B487-AE8898EA839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CB2729-A408-4A65-818F-C78917C13E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,16 +106,16 @@
     <t>Pengelola</t>
   </si>
   <si>
-    <t>dr.Hj.Sri Zakiah Usman</t>
-  </si>
-  <si>
     <t>Isdayana, SKM</t>
   </si>
   <si>
-    <t>Nip. 19700521 200212 2 006</t>
+    <t>Nip. 19801025 200604 2 028</t>
   </si>
   <si>
-    <t>Nip. 19801025 200604 2 028</t>
+    <t>dr. Fatimah, M.Kes</t>
+  </si>
+  <si>
+    <t>Nip. 19851125 201101 2 009</t>
   </si>
 </sst>
 </file>
@@ -462,23 +462,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -488,6 +488,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -500,15 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,33 +816,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:26" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="18"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -939,16 +939,16 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -960,21 +960,21 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="17" t="s">
+      <c r="N5" s="26"/>
+      <c r="O5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="17" t="s">
+      <c r="Q5" s="28"/>
+      <c r="R5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="S5" s="1"/>
@@ -987,44 +987,44 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="13" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="13" t="s">
+      <c r="O6" s="14"/>
+      <c r="P6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="18"/>
+      <c r="R6" s="14"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -1035,28 +1035,28 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="25" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1604,7 +1604,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="26" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1636,7 +1636,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -3724,6 +3724,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:R7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
@@ -3740,11 +3745,6 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>